<commit_message>
Upto 4 new bug
</commit_message>
<xml_diff>
--- a/api_handler_app/Habile_Investak_API_Dictionary_Local.xlsx
+++ b/api_handler_app/Habile_Investak_API_Dictionary_Local.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="20730" windowHeight="11760" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="20730" windowHeight="11760" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="8" r:id="rId1"/>
@@ -3950,6 +3950,9 @@
     <t>logout/</t>
   </si>
   <si>
+    <t>http://127.0.0.1:8000/</t>
+  </si>
+  <si>
     <t>N,Y</t>
   </si>
   <si>
@@ -3969,9 +3972,6 @@
   </si>
   <si>
     <t>Not_Ok,None</t>
-  </si>
-  <si>
-    <t>http://52.43.99.16:8000/</t>
   </si>
 </sst>
 </file>
@@ -9047,7 +9047,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J3" sqref="J3"/>
+      <selection pane="bottomRight" activeCell="K1" sqref="K1:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9128,7 +9128,7 @@
       <c r="I2" s="5"/>
       <c r="J2" s="12"/>
       <c r="K2" s="44" t="s">
-        <v>1291</v>
+        <v>1284</v>
       </c>
       <c r="L2" s="68" t="s">
         <v>1236</v>
@@ -9222,11 +9222,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P2" sqref="P2"/>
+      <selection pane="bottomRight" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12849,11 +12849,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P107"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E83" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G106" sqref="G106"/>
+      <selection pane="bottomRight" activeCell="H91" sqref="H91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14265,7 +14265,7 @@
         <v>63</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="I46" s="6" t="s">
         <v>1161</v>
@@ -19529,7 +19529,7 @@
         <v>947</v>
       </c>
       <c r="G126" s="78" t="s">
-        <v>1288</v>
+        <v>1289</v>
       </c>
       <c r="H126" s="78"/>
       <c r="I126" s="79"/>
@@ -22085,7 +22085,7 @@
         <v>11</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>1289</v>
+        <v>1290</v>
       </c>
       <c r="E223" s="1"/>
       <c r="F223" s="1"/>
@@ -22672,7 +22672,7 @@
         <v>63</v>
       </c>
       <c r="G25" s="21" t="s">
-        <v>1290</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="24">
@@ -27533,7 +27533,7 @@
         <v>54</v>
       </c>
       <c r="D134" s="72" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="E134" s="72"/>
       <c r="F134" s="72" t="s">
@@ -27552,7 +27552,7 @@
         <v>55</v>
       </c>
       <c r="D135" s="72" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
       <c r="E135" s="72"/>
       <c r="F135" s="72" t="s">
@@ -27571,7 +27571,7 @@
         <v>56</v>
       </c>
       <c r="D136" s="72" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
       <c r="E136" s="72"/>
       <c r="F136" s="72" t="s">

</xml_diff>